<commit_message>
final step (submission of project: success)
</commit_message>
<xml_diff>
--- a/Documentations/bayad 1.xlsx
+++ b/Documentations/bayad 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26A45B6-C23B-4E28-8786-67DE941136F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A40AD-38FB-47BE-A2DC-7660C99972F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>total abono</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>solder fee</t>
+  </si>
+  <si>
+    <t>battery (169)</t>
   </si>
 </sst>
 </file>
@@ -875,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA30" sqref="AA30"/>
+    <sheetView tabSelected="1" topLeftCell="K13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,23 +1152,23 @@
         <v>604.57142857142856</v>
       </c>
       <c r="X20" s="3">
-        <v>0</v>
+        <v>605</v>
       </c>
       <c r="Y20">
         <f t="shared" ref="Y20:Y26" si="2">W20-X20</f>
-        <v>604.57142857142856</v>
+        <v>-0.42857142857144481</v>
       </c>
       <c r="AA20">
-        <f>S20+W20</f>
+        <f t="shared" ref="AA20:AC26" si="3">S20+W20</f>
         <v>800.28571428571422</v>
       </c>
       <c r="AB20">
-        <f>T20+X20</f>
-        <v>200</v>
+        <f t="shared" si="3"/>
+        <v>805</v>
       </c>
       <c r="AC20">
-        <f>U20+Y20</f>
-        <v>600.28571428571422</v>
+        <f t="shared" si="3"/>
+        <v>-4.7142857142857224</v>
       </c>
     </row>
     <row r="21" spans="2:30" x14ac:dyDescent="0.3">
@@ -1203,20 +1206,20 @@
         <v>-3627.4285714285716</v>
       </c>
       <c r="AA21">
-        <f>S21+W21</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB21">
-        <f>T21+X21</f>
+        <f t="shared" si="3"/>
         <v>5122</v>
       </c>
       <c r="AC21">
-        <f>U21+Y21</f>
+        <f t="shared" si="3"/>
         <v>-4321.7142857142862</v>
       </c>
       <c r="AD21">
         <f>SUM(AC20:AC26)</f>
-        <v>-986.00000000000091</v>
+        <v>-3095</v>
       </c>
     </row>
     <row r="22" spans="2:30" x14ac:dyDescent="0.3">
@@ -1240,7 +1243,7 @@
         <v>190</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:U26" si="3">S22-T22</f>
+        <f t="shared" ref="U22:U26" si="4">S22-T22</f>
         <v>5.7142857142857224</v>
       </c>
       <c r="W22">
@@ -1255,15 +1258,15 @@
         <v>104.57142857142856</v>
       </c>
       <c r="AA22">
-        <f>S22+W22</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB22">
-        <f>T22+X22</f>
+        <f t="shared" si="3"/>
         <v>690</v>
       </c>
       <c r="AC22">
-        <f>U22+Y22</f>
+        <f t="shared" si="3"/>
         <v>110.28571428571428</v>
       </c>
     </row>
@@ -1291,7 +1294,7 @@
         <v>190</v>
       </c>
       <c r="U23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7142857142857224</v>
       </c>
       <c r="W23">
@@ -1306,15 +1309,15 @@
         <v>604.57142857142856</v>
       </c>
       <c r="AA23">
-        <f>S23+W23</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB23">
-        <f>T23+X23</f>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
       <c r="AC23">
-        <f>U23+Y23</f>
+        <f t="shared" si="3"/>
         <v>610.28571428571422</v>
       </c>
     </row>
@@ -1343,7 +1346,7 @@
         <v>190</v>
       </c>
       <c r="U24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7142857142857224</v>
       </c>
       <c r="W24">
@@ -1358,15 +1361,15 @@
         <v>604.57142857142856</v>
       </c>
       <c r="AA24">
-        <f>S24+W24</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB24">
-        <f>T24+X24</f>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
       <c r="AC24">
-        <f>U24+Y24</f>
+        <f t="shared" si="3"/>
         <v>610.28571428571422</v>
       </c>
     </row>
@@ -1397,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="U25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>195.71428571428572</v>
       </c>
       <c r="W25">
@@ -1405,23 +1408,23 @@
         <v>604.57142857142856</v>
       </c>
       <c r="X25" s="4">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="Y25">
         <f t="shared" si="2"/>
-        <v>604.57142857142856</v>
+        <v>-195.42857142857144</v>
       </c>
       <c r="AA25">
-        <f>S25+W25</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB25">
-        <f>T25+X25</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>800</v>
       </c>
       <c r="AC25">
-        <f>U25+Y25</f>
-        <v>800.28571428571422</v>
+        <f t="shared" si="3"/>
+        <v>0.28571428571427759</v>
       </c>
     </row>
     <row r="26" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1448,7 +1451,7 @@
         <v>196</v>
       </c>
       <c r="U26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-0.28571428571427759</v>
       </c>
       <c r="W26">
@@ -1456,23 +1459,24 @@
         <v>604.57142857142856</v>
       </c>
       <c r="X26" s="5">
-        <v>0</v>
+        <f>600+100+4</f>
+        <v>704</v>
       </c>
       <c r="Y26">
         <f t="shared" si="2"/>
-        <v>604.57142857142856</v>
+        <v>-99.428571428571445</v>
       </c>
       <c r="AA26">
-        <f>S26+W26</f>
+        <f t="shared" si="3"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AB26">
-        <f>T26+X26</f>
-        <v>196</v>
+        <f t="shared" si="3"/>
+        <v>900</v>
       </c>
       <c r="AC26">
-        <f>U26+Y26</f>
-        <v>604.28571428571422</v>
+        <f t="shared" si="3"/>
+        <v>-99.714285714285722</v>
       </c>
     </row>
     <row r="27" spans="2:30" x14ac:dyDescent="0.3">
@@ -1749,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="S36">
-        <f t="shared" ref="S36:S42" si="4">(G$4/7)</f>
+        <f t="shared" ref="S36:S42" si="5">(G$4/7)</f>
         <v>195.71428571428572</v>
       </c>
       <c r="T36" s="3">
@@ -1760,14 +1764,14 @@
         <v>0.71428571428572241</v>
       </c>
       <c r="W36">
-        <f t="shared" ref="W36:W42" si="5">($D$48/7)</f>
+        <f t="shared" ref="W36:W42" si="6">($D$48/7)</f>
         <v>604.57142857142856</v>
       </c>
       <c r="X36" s="3">
         <v>593</v>
       </c>
       <c r="Y36">
-        <f t="shared" ref="Y36" si="6">W36-X36</f>
+        <f t="shared" ref="Y36" si="7">W36-X36</f>
         <v>11.571428571428555</v>
       </c>
       <c r="AA36">
@@ -1815,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="S37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T37" s="4">
@@ -1827,7 +1831,7 @@
         <v>-694.28571428571422</v>
       </c>
       <c r="W37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X37" s="4">
@@ -1850,15 +1854,15 @@
         <v>-4372.7142857142862</v>
       </c>
       <c r="AE37">
-        <f t="shared" ref="AE37:AE42" si="7">S37+W37</f>
+        <f t="shared" ref="AE37:AE42" si="8">S37+W37</f>
         <v>800.28571428571422</v>
       </c>
       <c r="AF37">
-        <f t="shared" ref="AF37:AF42" si="8">T37+X37</f>
+        <f t="shared" ref="AF37:AF42" si="9">T37+X37</f>
         <v>5173</v>
       </c>
       <c r="AG37">
-        <f t="shared" ref="AG37:AG42" si="9">U37+Y37</f>
+        <f t="shared" ref="AG37:AG42" si="10">U37+Y37</f>
         <v>-4372.7142857142862</v>
       </c>
     </row>
@@ -1879,49 +1883,49 @@
         <v>7</v>
       </c>
       <c r="S38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T38" s="4">
         <v>195</v>
       </c>
       <c r="U38">
-        <f t="shared" ref="U38:U42" si="10">S38-T38</f>
+        <f t="shared" ref="U38:U42" si="11">S38-T38</f>
         <v>0.71428571428572241</v>
       </c>
       <c r="W38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X38" s="4">
         <v>593</v>
       </c>
       <c r="Y38">
-        <f t="shared" ref="Y38:Y42" si="11">W38-X38</f>
+        <f t="shared" ref="Y38:Y42" si="12">W38-X38</f>
         <v>11.571428571428555</v>
       </c>
       <c r="AA38">
-        <f t="shared" ref="AA38:AA42" si="12">U38+Y38</f>
+        <f t="shared" ref="AA38:AA42" si="13">U38+Y38</f>
         <v>12.285714285714278</v>
       </c>
       <c r="AB38">
-        <f t="shared" ref="AB38:AB42" si="13">T38+X38</f>
+        <f t="shared" ref="AB38:AB42" si="14">T38+X38</f>
         <v>788</v>
       </c>
       <c r="AC38">
-        <f t="shared" ref="AC38:AC42" si="14">U38+Y38</f>
+        <f t="shared" ref="AC38:AC42" si="15">U38+Y38</f>
         <v>12.285714285714278</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AF38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>788</v>
       </c>
       <c r="AG38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.285714285714278</v>
       </c>
     </row>
@@ -1935,55 +1939,59 @@
       <c r="D39">
         <v>102</v>
       </c>
-      <c r="M39" s="17"/>
-      <c r="O39" s="18"/>
+      <c r="M39" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O39" s="18">
+        <v>169</v>
+      </c>
       <c r="R39" t="s">
         <v>24</v>
       </c>
       <c r="S39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T39" s="4">
         <v>195</v>
       </c>
       <c r="U39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.71428571428572241</v>
       </c>
       <c r="W39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X39" s="4">
         <v>593</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.571428571428555</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>788</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AF39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>788</v>
       </c>
       <c r="AG39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.285714285714278</v>
       </c>
     </row>
@@ -2007,49 +2015,49 @@
         <v>8</v>
       </c>
       <c r="S40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T40" s="4">
         <v>195</v>
       </c>
       <c r="U40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.71428571428572241</v>
       </c>
       <c r="W40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X40" s="4">
         <v>593</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.571428571428555</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>788</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AE40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AF40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>788</v>
       </c>
       <c r="AG40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.285714285714278</v>
       </c>
     </row>
@@ -2064,55 +2072,55 @@
         <v>69</v>
       </c>
       <c r="O41" s="18">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="R41" t="s">
         <v>9</v>
       </c>
       <c r="S41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T41" s="4">
         <v>195</v>
       </c>
       <c r="U41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.71428571428572241</v>
       </c>
       <c r="W41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X41" s="4">
         <v>593</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.571428571428555</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>788</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>12.285714285714278</v>
       </c>
       <c r="AE41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AF41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>788</v>
       </c>
       <c r="AG41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>12.285714285714278</v>
       </c>
     </row>
@@ -2125,56 +2133,56 @@
       </c>
       <c r="M42" s="17"/>
       <c r="O42" s="12">
-        <f>SUM(O40:O41)</f>
-        <v>87</v>
+        <f>SUM(O39:O41)</f>
+        <v>275</v>
       </c>
       <c r="R42" t="s">
         <v>10</v>
       </c>
       <c r="S42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>195.71428571428572</v>
       </c>
       <c r="T42" s="5">
         <v>196</v>
       </c>
       <c r="U42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.28571428571427759</v>
       </c>
       <c r="W42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>604.57142857142856</v>
       </c>
       <c r="X42" s="5">
         <v>593</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.571428571428555</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11.285714285714278</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>789</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>11.285714285714278</v>
       </c>
       <c r="AE42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>800.28571428571422</v>
       </c>
       <c r="AF42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>789</v>
       </c>
       <c r="AG42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.285714285714278</v>
       </c>
     </row>
@@ -2234,19 +2242,19 @@
       <c r="M45" s="17"/>
       <c r="O45" s="13">
         <f>SUM(O42)+O37+O32+O26</f>
-        <v>1243.5</v>
+        <v>1431.5</v>
       </c>
       <c r="AA45">
-        <f>U20+Y20</f>
-        <v>600.28571428571422</v>
+        <f t="shared" ref="AA45:AA51" si="16">U20+Y20</f>
+        <v>-4.7142857142857224</v>
       </c>
       <c r="AB45">
-        <f>T20+X20</f>
-        <v>200</v>
+        <f t="shared" ref="AB45:AC51" si="17">T20+X20</f>
+        <v>805</v>
       </c>
       <c r="AC45">
-        <f>U20+Y20</f>
-        <v>600.28571428571422</v>
+        <f t="shared" si="17"/>
+        <v>-4.7142857142857224</v>
       </c>
     </row>
     <row r="46" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2260,15 +2268,15 @@
       <c r="N46" s="21"/>
       <c r="O46" s="22"/>
       <c r="AA46">
-        <f>U21+Y21</f>
+        <f t="shared" si="16"/>
         <v>-4321.7142857142862</v>
       </c>
       <c r="AB46">
-        <f>T21+X21</f>
+        <f t="shared" si="17"/>
         <v>5122</v>
       </c>
       <c r="AC46">
-        <f>U21+Y21</f>
+        <f t="shared" si="17"/>
         <v>-4321.7142857142862</v>
       </c>
     </row>
@@ -2280,15 +2288,15 @@
         <v>150</v>
       </c>
       <c r="AA47">
-        <f>U22+Y22</f>
+        <f t="shared" si="16"/>
         <v>110.28571428571428</v>
       </c>
       <c r="AB47">
-        <f>T22+X22</f>
+        <f t="shared" si="17"/>
         <v>690</v>
       </c>
       <c r="AC47">
-        <f>U22+Y22</f>
+        <f t="shared" si="17"/>
         <v>110.28571428571428</v>
       </c>
     </row>
@@ -2302,15 +2310,15 @@
         <v>3023.5</v>
       </c>
       <c r="AA48">
-        <f>U23+Y23</f>
+        <f t="shared" si="16"/>
         <v>610.28571428571422</v>
       </c>
       <c r="AB48">
-        <f>T23+X23</f>
+        <f t="shared" si="17"/>
         <v>190</v>
       </c>
       <c r="AC48">
-        <f>U23+Y23</f>
+        <f t="shared" si="17"/>
         <v>610.28571428571422</v>
       </c>
     </row>
@@ -2325,15 +2333,15 @@
         <v>20</v>
       </c>
       <c r="AA49">
-        <f>U24+Y24</f>
+        <f t="shared" si="16"/>
         <v>610.28571428571422</v>
       </c>
       <c r="AB49">
-        <f>T24+X24</f>
+        <f t="shared" si="17"/>
         <v>190</v>
       </c>
       <c r="AC49">
-        <f>U24+Y24</f>
+        <f t="shared" si="17"/>
         <v>610.28571428571422</v>
       </c>
     </row>
@@ -2351,16 +2359,16 @@
         <v>800.28571428571433</v>
       </c>
       <c r="AA50">
-        <f>U25+Y25</f>
-        <v>800.28571428571422</v>
+        <f t="shared" si="16"/>
+        <v>0.28571428571427759</v>
       </c>
       <c r="AB50">
-        <f>T25+X25</f>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>800</v>
       </c>
       <c r="AC50">
-        <f>U25+Y25</f>
-        <v>800.28571428571422</v>
+        <f t="shared" si="17"/>
+        <v>0.28571428571427759</v>
       </c>
     </row>
     <row r="51" spans="3:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2372,16 +2380,16 @@
         <v>5602</v>
       </c>
       <c r="AA51">
-        <f>U26+Y26</f>
-        <v>604.28571428571422</v>
+        <f t="shared" si="16"/>
+        <v>-99.714285714285722</v>
       </c>
       <c r="AB51">
-        <f>T26+X26</f>
-        <v>196</v>
+        <f t="shared" si="17"/>
+        <v>900</v>
       </c>
       <c r="AC51">
-        <f>U26+Y26</f>
-        <v>604.28571428571422</v>
+        <f t="shared" si="17"/>
+        <v>-99.714285714285722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>